<commit_message>
Cleaning code, and new funcionalities
Search for expenses procedure and executables procedures
</commit_message>
<xml_diff>
--- a/sources/Planilha de Críticas.xlsx
+++ b/sources/Planilha de Críticas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliasp\Documents\GitHub\python-automatics-data-alterations-in-xml-file\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607336E2-8313-46E0-918A-267283317564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02C10A5-87F0-4C3B-9120-B7733CB81B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2610" windowWidth="15375" windowHeight="8160" activeTab="1" xr2:uid="{2CB27820-A556-4FB3-A9D8-7569D697D985}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2CB27820-A556-4FB3-A9D8-7569D697D985}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="2" r:id="rId1"/>
@@ -37,49 +37,142 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t>nr_conta</t>
-  </si>
-  <si>
-    <t>old_cod</t>
-  </si>
-  <si>
-    <t>new_cod</t>
-  </si>
-  <si>
-    <t>old_tipoT</t>
-  </si>
-  <si>
-    <t>new_tipoT</t>
-  </si>
-  <si>
-    <t>old_unidM</t>
-  </si>
-  <si>
-    <t>new_unidM</t>
-  </si>
-  <si>
-    <t>cod</t>
-  </si>
-  <si>
-    <t>old_vlr</t>
-  </si>
-  <si>
-    <t>new_vlr</t>
-  </si>
-  <si>
-    <t>88787997</t>
-  </si>
-  <si>
-    <t>888888888</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+  <si>
+    <t>Número da conta</t>
+  </si>
+  <si>
+    <t>Código do procedimento</t>
+  </si>
+  <si>
+    <t>Valor unitário (atual)</t>
+  </si>
+  <si>
+    <t>Valor unitário (novo)</t>
+  </si>
+  <si>
+    <t>Código do procedimento (atual)</t>
+  </si>
+  <si>
+    <t>Código do procedimento (novo)</t>
+  </si>
+  <si>
+    <t>Tipo de tabela (atual)</t>
+  </si>
+  <si>
+    <t>Tipo de tabela (novo)</t>
+  </si>
+  <si>
+    <t>Unidade de medida (atual)</t>
+  </si>
+  <si>
+    <t>Unidade de medida (novo)</t>
+  </si>
+  <si>
+    <t>0000062684</t>
+  </si>
+  <si>
+    <t>2094000492</t>
+  </si>
+  <si>
+    <t>79419623</t>
+  </si>
+  <si>
+    <t>1900159085</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>0000119306</t>
+  </si>
+  <si>
+    <t>1900224723</t>
+  </si>
+  <si>
+    <t>0000145371</t>
+  </si>
+  <si>
+    <t>1902962543</t>
+  </si>
+  <si>
+    <t>0000767118</t>
+  </si>
+  <si>
+    <t>1900312770</t>
+  </si>
+  <si>
+    <t>78202426</t>
+  </si>
+  <si>
+    <t>1900774243</t>
+  </si>
+  <si>
+    <t>0000273887</t>
+  </si>
+  <si>
+    <t>1900405140</t>
+  </si>
+  <si>
+    <t>78413494</t>
+  </si>
+  <si>
+    <t>1900108332</t>
+  </si>
+  <si>
+    <t>0000064026</t>
+  </si>
+  <si>
+    <t>90247604</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>0000306686</t>
+  </si>
+  <si>
+    <t>2094372470</t>
+  </si>
+  <si>
+    <t>60002054</t>
+  </si>
+  <si>
+    <t>60001054</t>
+  </si>
+  <si>
+    <t>70705259</t>
+  </si>
+  <si>
+    <t>1900225495</t>
+  </si>
+  <si>
+    <t>78213061</t>
+  </si>
+  <si>
+    <t>1900051101</t>
+  </si>
+  <si>
+    <t>78216036</t>
+  </si>
+  <si>
+    <t>1900167800</t>
+  </si>
+  <si>
+    <t>78269423</t>
+  </si>
+  <si>
+    <t>1900488682</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,30 +187,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color rgb="FF535353"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF535353"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0E0E0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,27 +216,18 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -171,6 +243,24 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -205,29 +295,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}" name="Tabela13" displayName="Tabela13" ref="A1:G2" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowCellStyle="Normal" dataCellStyle="Normal">
-  <autoFilter ref="A1:G2" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}" name="Tabela13" displayName="Tabela13" ref="A1:G19" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13" headerRowCellStyle="Normal" dataCellStyle="Normal">
+  <autoFilter ref="A1:G19" xr:uid="{85B1F556-4732-4418-B94B-898810A3A352}"/>
   <tableColumns count="7">
-    <tableColumn id="13" xr3:uid="{76A2E480-B71B-42BF-8C12-04854B133A08}" name="nr_conta" dataDxfId="9" dataCellStyle="Normal"/>
-    <tableColumn id="1" xr3:uid="{1C128478-DCB8-4EE0-A2EA-0179F6564A25}" name="old_cod" dataDxfId="8" dataCellStyle="Normal"/>
-    <tableColumn id="2" xr3:uid="{192DAD45-D9CC-4B01-867D-AE4BCC975DAB}" name="new_cod" dataDxfId="7" dataCellStyle="Normal"/>
-    <tableColumn id="3" xr3:uid="{892B31F4-BDAF-4D4F-BB11-95B930583EEB}" name="old_tipoT" dataDxfId="6" dataCellStyle="Normal"/>
-    <tableColumn id="4" xr3:uid="{0DC4EA1C-95C4-4E67-8D90-26BAA3E071F8}" name="new_tipoT" dataDxfId="5" dataCellStyle="Normal"/>
-    <tableColumn id="11" xr3:uid="{653771AE-85CB-4906-A207-14B15DE69D6F}" name="old_unidM" dataDxfId="4" dataCellStyle="Normal"/>
-    <tableColumn id="12" xr3:uid="{25FF0592-2163-461B-83C0-A568FE200326}" name="new_unidM" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{76A2E480-B71B-42BF-8C12-04854B133A08}" name="Número da conta" dataDxfId="12" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{1C128478-DCB8-4EE0-A2EA-0179F6564A25}" name="Código do procedimento (atual)" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{192DAD45-D9CC-4B01-867D-AE4BCC975DAB}" name="Código do procedimento (novo)" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{892B31F4-BDAF-4D4F-BB11-95B930583EEB}" name="Tipo de tabela (atual)" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{0DC4EA1C-95C4-4E67-8D90-26BAA3E071F8}" name="Tipo de tabela (novo)" dataDxfId="0" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{653771AE-85CB-4906-A207-14B15DE69D6F}" name="Unidade de medida (atual)" dataDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{25FF0592-2163-461B-83C0-A568FE200326}" name="Unidade de medida (novo)" dataDxfId="10" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}" name="Tabela3" displayName="Tabela3" ref="A1:D2" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:D2" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}" name="Tabela3" displayName="Tabela3" ref="A1:D8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:D8" xr:uid="{EF3F8EE2-2535-4055-995F-58277DA69320}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E041450B-B9A8-4984-80F1-F392EA1249E0}" name="nr_conta" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{34DF0F1F-4A50-4495-9A62-004334AB22FA}" name="cod"/>
-    <tableColumn id="3" xr3:uid="{AA7D6B72-0CFC-4D03-95C6-61EB48D14747}" name="old_vlr"/>
-    <tableColumn id="4" xr3:uid="{3D107E8F-238F-4D9E-A978-F4020F61C26E}" name="new_vlr"/>
+    <tableColumn id="1" xr3:uid="{E041450B-B9A8-4984-80F1-F392EA1249E0}" name="Número da conta" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{34DF0F1F-4A50-4495-9A62-004334AB22FA}" name="Código do procedimento" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{AA7D6B72-0CFC-4D03-95C6-61EB48D14747}" name="Valor unitário (atual)" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3D107E8F-238F-4D9E-A978-F4020F61C26E}" name="Valor unitário (novo)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -530,21 +620,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C61B51D-8349-4064-B6F9-68B2ADB2D555}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="32.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -553,35 +640,266 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -597,16 +915,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{659A0C52-99B9-496E-B347-5D1AC694609B}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="14" max="14" width="43.42578125" customWidth="1"/>
     <col min="15" max="15" width="37.85546875" customWidth="1"/>
@@ -621,26 +938,56 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="2">
-        <v>88787997</v>
-      </c>
-      <c r="C2" s="2">
-        <v>9.16</v>
-      </c>
-      <c r="D2" s="2">
-        <v>10</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S13" t="str">

</xml_diff>